<commit_message>
xóa cột Tổng cộng
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_PhanTichThuChiTheoNam.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_PhanTichThuChiTheoNam.xlsx
@@ -12,17 +12,14 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Tổng</t>
-  </si>
-  <si>
-    <t>Năm</t>
   </si>
   <si>
     <t>BÁO CÁO PHÂN TÍCH THU CHI THEO NĂM</t>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -138,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -166,20 +163,17 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -486,238 +480,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="22.140625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15">
-        <f>B5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15">
-        <f t="shared" ref="C6:C27" si="0">B6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+    </row>
+    <row r="24" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>